<commit_message>
Create USer TestScript is modified
</commit_message>
<xml_diff>
--- a/ActiTime/src/test/resources/result/report.xlsx
+++ b/ActiTime/src/test/resources/result/report.xlsx
@@ -1336,10 +1336,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>